<commit_message>
Excel file Reordered and data sorted
</commit_message>
<xml_diff>
--- a/src/data/input/examData/ExamData.xlsx
+++ b/src/data/input/examData/ExamData.xlsx
@@ -1,455 +1,347 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="a" sheetId="1" r:id="rId2"/>
+    <sheet name="a" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+  <si>
+    <t>Course Name</t>
+  </si>
   <si>
     <t>Course ID</t>
   </si>
   <si>
-    <t>Course Name</t>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>No of Students</t>
   </si>
   <si>
     <t>Batch Code</t>
   </si>
   <si>
-    <t>No of Students</t>
-  </si>
-  <si>
-    <t>Faculty</t>
+    <t>Digital Logic Design</t>
   </si>
   <si>
     <t>EL114</t>
   </si>
   <si>
-    <t>Digital Logic Design</t>
-  </si>
-  <si>
     <t>FFF</t>
   </si>
   <si>
+    <t>Analog Circuits</t>
+  </si>
+  <si>
     <t>EL213</t>
   </si>
   <si>
-    <t>Analog Circuits</t>
+    <t>Digital System Architecture (GE)</t>
   </si>
   <si>
     <t>EL426</t>
   </si>
   <si>
-    <t>Digital System Architecture (GE)</t>
+    <t>Internet of Things</t>
   </si>
   <si>
     <t>IT478</t>
   </si>
   <si>
-    <t>Internet of Things</t>
+    <t>Computational Electromagnetics</t>
   </si>
   <si>
     <t>IT483</t>
   </si>
   <si>
-    <t>Computational Electromagnetics</t>
+    <t>Detection and Estimation Theory</t>
   </si>
   <si>
     <t>CT513</t>
   </si>
   <si>
-    <t>Detection and Estimation Theory</t>
+    <t>Adv. Logic for Computer Science</t>
   </si>
   <si>
     <t>IT543</t>
   </si>
   <si>
-    <t>Adv. Logic for Computer Science</t>
+    <t>Enterprise Computing</t>
   </si>
   <si>
     <t>IT618</t>
   </si>
   <si>
-    <t>Enterprise Computing</t>
+    <t>Environmental Studies</t>
   </si>
   <si>
     <t>SC209</t>
   </si>
   <si>
-    <t>Environmental Studies</t>
+    <t>Analysis of Multi-Disciplinary Problems</t>
   </si>
   <si>
     <t>SC465</t>
   </si>
   <si>
-    <t>Analysis of Multi-Disciplinary Problems</t>
+    <t>Introduction to Narratology</t>
   </si>
   <si>
     <t>PC725</t>
   </si>
   <si>
-    <t>Introduction to Narratology</t>
+    <t>Digital Image Processing</t>
   </si>
   <si>
     <t>IT523</t>
   </si>
   <si>
-    <t>Digital Image Processing</t>
+    <t>Discrete Mathematics</t>
   </si>
   <si>
     <t>SC205</t>
   </si>
   <si>
-    <t>Discrete Mathematics</t>
+    <t>Probability and Statistics</t>
   </si>
   <si>
     <t>SC215</t>
   </si>
   <si>
-    <t>Probability and Statistics</t>
+    <t>Remote Sensing and GIS</t>
   </si>
   <si>
     <t>IT664</t>
   </si>
   <si>
-    <t>Remote Sensing and GIS</t>
+    <t>Software Engineering</t>
   </si>
   <si>
     <t>IT314</t>
   </si>
   <si>
-    <t>Software Engineering</t>
+    <t>Data Structures</t>
   </si>
   <si>
     <t>IT205</t>
   </si>
   <si>
-    <t>Data Structures</t>
+    <t>Systems Software</t>
   </si>
   <si>
     <t>IT215</t>
   </si>
   <si>
-    <t>Systems Software</t>
+    <t>Solid State Devices</t>
   </si>
   <si>
     <t>EL312</t>
   </si>
   <si>
-    <t>Solid State Devices</t>
+    <t>Introduction to Nonlinear Science</t>
   </si>
   <si>
     <t>CS304</t>
   </si>
   <si>
-    <t>Introduction to Nonlinear Science</t>
+    <t>Communications Skills</t>
   </si>
   <si>
     <t>HM501</t>
   </si>
   <si>
-    <t>Communications Skills</t>
+    <t>Operating Systems</t>
   </si>
   <si>
     <t>IT617</t>
   </si>
   <si>
-    <t>Operating Systems</t>
+    <t>Analog and Digital Communication</t>
   </si>
   <si>
     <t>CT214</t>
   </si>
   <si>
-    <t>Analog and Digital Communication</t>
+    <t>Statistical Communication Theory (GE)</t>
   </si>
   <si>
     <t>CT314</t>
   </si>
   <si>
-    <t>Statistical Communication Theory (GE)</t>
+    <t>Introduction to Quantum Mechanics</t>
   </si>
   <si>
     <t>SC332</t>
   </si>
   <si>
-    <t>Introduction to Quantum Mechanics</t>
+    <t>Web Data Management</t>
   </si>
   <si>
     <t>IT410</t>
   </si>
   <si>
-    <t>Web Data Management</t>
+    <t>Information Theory and Coding</t>
   </si>
   <si>
     <t>CT512</t>
   </si>
   <si>
-    <t>Information Theory and Coding</t>
+    <t>Analysis &amp; Design of Algorithms</t>
   </si>
   <si>
     <t>IT616</t>
   </si>
   <si>
-    <t>Analysis &amp; Design of Algorithms</t>
+    <t>Introduction to Nanoscience and Tech.</t>
   </si>
   <si>
     <t>SC431</t>
   </si>
   <si>
-    <t>Introduction to Nanoscience and Tech.</t>
+    <t>Software Testing and Quality Analysis</t>
   </si>
   <si>
     <t>IT415</t>
   </si>
   <si>
-    <t>Software Testing and Quality Analysis</t>
+    <t>Modeling and Simulation</t>
   </si>
   <si>
     <t>CS302</t>
   </si>
   <si>
-    <t>Modeling and Simulation</t>
+    <t>Graph Theory and Algorithms</t>
   </si>
   <si>
     <t>SC522</t>
   </si>
   <si>
-    <t>Graph Theory and Algorithms</t>
+    <t>Digital System Design using Verilog</t>
   </si>
   <si>
     <t>EL520</t>
   </si>
   <si>
-    <t>Digital System Design using Verilog</t>
+    <t>Computer Networks</t>
   </si>
   <si>
     <t>IT694</t>
   </si>
   <si>
-    <t>Computer Networks</t>
+    <t>Introductory Computational Physics (CS only)</t>
   </si>
   <si>
     <t>CS201</t>
   </si>
   <si>
-    <t>Introductory Computational Physics (CS only)</t>
+    <t>Advanced Digital Communications</t>
   </si>
   <si>
     <t>CT516</t>
   </si>
   <si>
-    <t>Advanced Digital Communications</t>
+    <t>Analog CMOS IC Design</t>
   </si>
   <si>
     <t>EL516</t>
   </si>
   <si>
-    <t>Analog CMOS IC Design</t>
+    <t>Systems Approach to Sustainable Development</t>
   </si>
   <si>
     <t>ES662</t>
   </si>
   <si>
-    <t>Systems Approach to Sustainable Development</t>
+    <t>Models of Computation</t>
   </si>
   <si>
     <t>IT422</t>
   </si>
   <si>
-    <t>Models of Computation</t>
+    <t>Introduction to Cryptology</t>
   </si>
   <si>
     <t>IT325</t>
   </si>
   <si>
-    <t>Introduction to Cryptology</t>
+    <t>Natural Computing</t>
   </si>
   <si>
     <t>IT468</t>
   </si>
   <si>
-    <t>Natural Computing</t>
+    <t>Operating System</t>
   </si>
   <si>
     <t>IT308</t>
   </si>
   <si>
-    <t>Operating System</t>
+    <t>Design of Software Systems</t>
   </si>
   <si>
     <t>IT619</t>
-  </si>
-  <si>
-    <t>Design of Software Systems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
   <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment/>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Comma" xfId="15"/>
-    <cellStyle name="Comma [0]" xfId="16"/>
-    <cellStyle name="Currency" xfId="17"/>
-    <cellStyle name="Currency [0]" xfId="18"/>
-    <cellStyle name="Percent" xfId="19"/>
-    <cellStyle name="Comma" xfId="20"/>
-    <cellStyle name="Comma [0]" xfId="21"/>
-    <cellStyle name="Currency" xfId="22"/>
-    <cellStyle name="Currency [0]" xfId="23"/>
-    <cellStyle name="Normal" xfId="24"/>
-    <cellStyle name="Percent" xfId="25"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -528,6 +420,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -562,6 +455,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -596,16 +490,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -727,85 +625,59 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A26">
-      <selection pane="topLeft" activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="12.75" defaultColWidth="8.72265625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.71428571428571" customWidth="1"/>
-    <col min="2" max="2" width="28.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="43.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="8.71428571428571" customWidth="1"/>
-    <col min="6" max="10" width="4.42857142857143" customWidth="1"/>
-    <col min="11" max="11" width="8.71428571428571" customWidth="1"/>
-    <col min="12" max="12" width="6.71428571428571" customWidth="1"/>
-    <col min="13" max="13" width="30.7142857142857" customWidth="1"/>
-    <col min="14" max="14" width="8.71428571428571" customWidth="1"/>
-    <col min="15" max="19" width="4.42857142857143" customWidth="1"/>
-    <col min="20" max="20" width="8.71428571428571" customWidth="1"/>
-    <col min="21" max="21" width="6.71428571428571" customWidth="1"/>
-    <col min="22" max="22" width="36" customWidth="1"/>
-    <col min="23" max="23" width="8.71428571428571" customWidth="1"/>
-    <col min="24" max="28" width="4.42857142857143" customWidth="1"/>
-    <col min="29" max="29" width="8.71428571428571" customWidth="1"/>
-    <col min="30" max="30" width="7.71428571428571" customWidth="1"/>
-    <col min="31" max="31" width="31.2857142857143" customWidth="1"/>
-    <col min="32" max="32" width="8.71428571428571" customWidth="1"/>
-    <col min="33" max="37" width="4.42857142857143" customWidth="1"/>
-    <col min="38" max="16384" width="8.71428571428571" customWidth="1"/>
+    <col min="1" max="1" width="28.60546875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="8.72265625" style="0"/>
+    <col min="3" max="3" width="8.72265625" style="0"/>
+    <col min="4" max="4" width="43.62109375" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13.15234375" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8.72265625" style="0"/>
+    <col min="7" max="7" width="6.72265625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="30.74609375" customWidth="true" style="0"/>
+    <col min="9" max="9" width="8.72265625" style="0"/>
+    <col min="10" max="10" width="4.43359375" customWidth="true" style="0"/>
+    <col min="11" max="11" width="4.43359375" customWidth="true" style="0"/>
+    <col min="12" max="12" width="4.43359375" customWidth="true" style="0"/>
+    <col min="13" max="13" width="4.43359375" customWidth="true" style="0"/>
+    <col min="14" max="14" width="4.43359375" customWidth="true" style="0"/>
+    <col min="15" max="15" width="8.72265625" style="0"/>
+    <col min="16" max="16" width="6.72265625" customWidth="true" style="0"/>
+    <col min="17" max="17" width="36.03515625" customWidth="true" style="0"/>
+    <col min="18" max="18" width="8.72265625" style="0"/>
+    <col min="19" max="19" width="4.43359375" customWidth="true" style="0"/>
+    <col min="20" max="20" width="4.43359375" customWidth="true" style="0"/>
+    <col min="21" max="21" width="4.43359375" customWidth="true" style="0"/>
+    <col min="22" max="22" width="4.43359375" customWidth="true" style="0"/>
+    <col min="23" max="23" width="4.43359375" customWidth="true" style="0"/>
+    <col min="24" max="24" width="8.72265625" style="0"/>
+    <col min="25" max="25" width="7.72265625" customWidth="true" style="0"/>
+    <col min="26" max="26" width="31.31640625" customWidth="true" style="0"/>
+    <col min="27" max="27" width="8.72265625" style="0"/>
+    <col min="28" max="28" width="4.43359375" customWidth="true" style="0"/>
+    <col min="29" max="29" width="4.43359375" customWidth="true" style="0"/>
+    <col min="30" max="30" width="4.43359375" customWidth="true" style="0"/>
+    <col min="31" max="31" width="4.43359375" customWidth="true" style="0"/>
+    <col min="32" max="32" width="4.43359375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75">
+    <row r="1" spans="1:32" customHeight="1" ht="12.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -822,741 +694,749 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75">
+    <row r="2" spans="1:32" customHeight="1" ht="12.75">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
         <v>311</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" customHeight="1" ht="12.75">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3">
         <v>302</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" customHeight="1" ht="12.75">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" customHeight="1" ht="12.75">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>3</v>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
       <c r="D5">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" customHeight="1" ht="12.75">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75">
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" customHeight="1" ht="12.75">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
-        <v>9</v>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75">
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" customHeight="1" ht="12.75">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>9</v>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
       <c r="D8">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75">
+      <c r="E8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" customHeight="1" ht="12.75">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
-        <v>5</v>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
       <c r="D9">
         <v>112</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75">
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" customHeight="1" ht="12.75">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>7</v>
       </c>
       <c r="D10">
         <v>297</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="12.75">
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" customHeight="1" ht="12.75">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>3</v>
+      <c r="C11" t="s">
+        <v>7</v>
       </c>
       <c r="D11">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75">
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" customHeight="1" ht="12.75">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>11</v>
+      <c r="C12" t="s">
+        <v>7</v>
       </c>
       <c r="D12">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75">
+      <c r="E12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" customHeight="1" ht="12.75">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13">
-        <v>9</v>
+      <c r="C13" t="s">
+        <v>7</v>
       </c>
       <c r="D13">
         <v>14</v>
       </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.75">
+      <c r="E13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" customHeight="1" ht="12.75">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>7</v>
       </c>
       <c r="D14">
         <v>310</v>
       </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="12.75">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" customHeight="1" ht="12.75">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C15">
-        <v>2</v>
+      <c r="C15" t="s">
+        <v>7</v>
       </c>
       <c r="D15">
         <v>296</v>
       </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" customHeight="1" ht="12.75">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="12.75">
+      <c r="E16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" customHeight="1" ht="12.75">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C17">
-        <v>3</v>
+      <c r="C17" t="s">
+        <v>7</v>
       </c>
       <c r="D17">
         <v>277</v>
       </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75">
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" customHeight="1" ht="12.75">
       <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>7</v>
       </c>
       <c r="D18">
         <v>309</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.75">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" customHeight="1" ht="12.75">
       <c r="A19" t="s">
         <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19">
-        <v>2</v>
+      <c r="C19" t="s">
+        <v>7</v>
       </c>
       <c r="D19">
         <v>298</v>
       </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75">
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" customHeight="1" ht="12.75">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C20">
-        <v>3</v>
+      <c r="C20" t="s">
+        <v>7</v>
       </c>
       <c r="D20">
         <v>40</v>
       </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="12.75">
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" customHeight="1" ht="12.75">
       <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21">
-        <v>3</v>
+      <c r="C21" t="s">
+        <v>7</v>
       </c>
       <c r="D21">
         <v>48</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75">
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" customHeight="1" ht="12.75">
       <c r="A22" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C22">
-        <v>9</v>
+      <c r="C22" t="s">
+        <v>7</v>
       </c>
       <c r="D22">
         <v>70</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="12.75">
+      <c r="E22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" customHeight="1" ht="12.75">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="C23">
-        <v>5</v>
+      <c r="C23" t="s">
+        <v>7</v>
       </c>
       <c r="D23">
         <v>113</v>
       </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.75">
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" customHeight="1" ht="12.75">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24">
-        <v>2</v>
+      <c r="C24" t="s">
+        <v>7</v>
       </c>
       <c r="D24">
         <v>297</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="12.75">
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" customHeight="1" ht="12.75">
       <c r="A25" t="s">
         <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25">
-        <v>3</v>
+      <c r="C25" t="s">
+        <v>7</v>
       </c>
       <c r="D25">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="12.75">
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" customHeight="1" ht="12.75">
       <c r="A26" t="s">
         <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="C26">
-        <v>3</v>
+      <c r="C26" t="s">
+        <v>7</v>
       </c>
       <c r="D26">
         <v>61</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="12.75">
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" customHeight="1" ht="12.75">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C27">
-        <v>9</v>
+      <c r="C27" t="s">
+        <v>7</v>
       </c>
       <c r="D27">
         <v>11</v>
       </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="12.75">
+      <c r="E27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" customHeight="1" ht="12.75">
       <c r="A28" t="s">
         <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="C28">
-        <v>9</v>
+      <c r="C28" t="s">
+        <v>7</v>
       </c>
       <c r="D28">
         <v>12</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="12.75">
+      <c r="E28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" customHeight="1" ht="12.75">
       <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C29">
-        <v>5</v>
+      <c r="C29" t="s">
+        <v>7</v>
       </c>
       <c r="D29">
         <v>109</v>
       </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="12.75">
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" customHeight="1" ht="12.75">
       <c r="A30" t="s">
         <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="C30">
-        <v>3</v>
+      <c r="C30" t="s">
+        <v>7</v>
       </c>
       <c r="D30">
         <v>64</v>
       </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="12.75">
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" customHeight="1" ht="12.75">
       <c r="A31" t="s">
         <v>64</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C31">
-        <v>3</v>
+      <c r="C31" t="s">
+        <v>7</v>
       </c>
       <c r="D31">
         <v>163</v>
       </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="12.75">
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" customHeight="1" ht="12.75">
       <c r="A32" t="s">
         <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="C32">
-        <v>3</v>
+      <c r="C32" t="s">
+        <v>7</v>
       </c>
       <c r="D32">
         <v>55</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="12.75">
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" customHeight="1" ht="12.75">
       <c r="A33" t="s">
         <v>68</v>
       </c>
       <c r="B33" t="s">
         <v>69</v>
       </c>
-      <c r="C33">
-        <v>9</v>
+      <c r="C33" t="s">
+        <v>7</v>
       </c>
       <c r="D33">
         <v>26</v>
       </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="12.75">
+      <c r="E33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" customHeight="1" ht="12.75">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>71</v>
       </c>
-      <c r="C34">
-        <v>9</v>
+      <c r="C34" t="s">
+        <v>7</v>
       </c>
       <c r="D34">
         <v>15</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="12.75">
+      <c r="E34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" customHeight="1" ht="12.75">
       <c r="A35" t="s">
         <v>72</v>
       </c>
       <c r="B35" t="s">
         <v>73</v>
       </c>
-      <c r="C35">
-        <v>5</v>
+      <c r="C35" t="s">
+        <v>7</v>
       </c>
       <c r="D35">
         <v>109</v>
       </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="12.75">
+      <c r="E35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" customHeight="1" ht="12.75">
       <c r="A36" t="s">
         <v>74</v>
       </c>
       <c r="B36" t="s">
         <v>75</v>
       </c>
-      <c r="C36">
-        <v>2</v>
+      <c r="C36" t="s">
+        <v>7</v>
       </c>
       <c r="D36">
         <v>56</v>
       </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="12.75">
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" customHeight="1" ht="12.75">
       <c r="A37" t="s">
         <v>76</v>
       </c>
       <c r="B37" t="s">
         <v>77</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
         <v>9</v>
       </c>
-      <c r="D37">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="12.75">
+    </row>
+    <row r="38" spans="1:32" customHeight="1" ht="12.75">
       <c r="A38" t="s">
         <v>78</v>
       </c>
       <c r="B38" t="s">
         <v>79</v>
       </c>
-      <c r="C38">
-        <v>9</v>
+      <c r="C38" t="s">
+        <v>7</v>
       </c>
       <c r="D38">
         <v>13</v>
       </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="12.75">
+      <c r="E38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" customHeight="1" ht="12.75">
       <c r="A39" t="s">
         <v>80</v>
       </c>
       <c r="B39" t="s">
         <v>81</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="12.75">
+      <c r="E39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" customHeight="1" ht="12.75">
       <c r="A40" t="s">
         <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="C40">
-        <v>3</v>
+      <c r="C40" t="s">
+        <v>7</v>
       </c>
       <c r="D40">
         <v>136</v>
       </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="12.75">
+      <c r="E40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" customHeight="1" ht="12.75">
       <c r="A41" t="s">
         <v>84</v>
       </c>
       <c r="B41" t="s">
         <v>85</v>
       </c>
-      <c r="C41">
-        <v>3</v>
+      <c r="C41" t="s">
+        <v>7</v>
       </c>
       <c r="D41">
         <v>112</v>
       </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="12.75">
+      <c r="E41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" customHeight="1" ht="12.75">
       <c r="A42" t="s">
         <v>86</v>
       </c>
       <c r="B42" t="s">
         <v>87</v>
       </c>
-      <c r="C42">
-        <v>3</v>
+      <c r="C42" t="s">
+        <v>7</v>
       </c>
       <c r="D42">
         <v>38</v>
       </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="12.75">
+      <c r="E42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" customHeight="1" ht="12.75">
       <c r="A43" t="s">
         <v>88</v>
       </c>
       <c r="B43" t="s">
         <v>89</v>
       </c>
-      <c r="C43">
-        <v>3</v>
+      <c r="C43" t="s">
+        <v>7</v>
       </c>
       <c r="D43">
         <v>241</v>
       </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="12.75">
+      <c r="E43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" customHeight="1" ht="12.75">
       <c r="A44" t="s">
         <v>90</v>
       </c>
       <c r="B44" t="s">
         <v>91</v>
       </c>
-      <c r="C44">
-        <v>5</v>
+      <c r="C44" t="s">
+        <v>7</v>
       </c>
       <c r="D44">
         <v>109</v>
       </c>
-      <c r="E44" t="s">
-        <v>7</v>
+      <c r="E44">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="landscape" paperSize="1"/>
-  <headerFooter alignWithMargins="0"/>
+  <sheetProtection sheet="false" objects="true" scenarios="true" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="true" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="true"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555556" footer="0.51180555555556"/>
+  <pageSetup paperSize="1" orientation="landscape" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>